<commit_message>
Use ClosedXML for Excel
</commit_message>
<xml_diff>
--- a/Parser/listAlert.xlsx
+++ b/Parser/listAlert.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Azizbek\Desktop\Education Projects\Parser\Parser\Parser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C3AB87B1-8D58-48AB-8144-D7A4197D7E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{88825F46-E65A-499F-BC6B-B88EE4D58802}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6540" yWindow="4095" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>

</xml_diff>